<commit_message>
update notebooks and presentation
</commit_message>
<xml_diff>
--- a/Datasets/chords.xlsx
+++ b/Datasets/chords.xlsx
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -1415,7 +1415,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1685,7 +1685,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -1901,7 +1901,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2243,7 +2243,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -2423,7 +2423,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -2531,7 +2531,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
@@ -2729,7 +2729,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
@@ -2927,7 +2927,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
@@ -2981,7 +2981,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
@@ -2999,7 +2999,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
@@ -3737,7 +3737,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D184" t="inlineStr">
         <is>
@@ -3863,7 +3863,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="D191" t="inlineStr">
         <is>
@@ -4025,7 +4025,7 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D200" t="inlineStr">
         <is>
@@ -4097,7 +4097,7 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D204" t="inlineStr">
         <is>
@@ -4295,7 +4295,7 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D215" t="inlineStr">
         <is>
@@ -4583,7 +4583,7 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D231" t="inlineStr">
         <is>
@@ -5141,7 +5141,7 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D262" t="inlineStr">
         <is>
@@ -5267,7 +5267,7 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D269" t="inlineStr">
         <is>
@@ -5411,7 +5411,7 @@
         </is>
       </c>
       <c r="C277" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D277" t="inlineStr">
         <is>
@@ -5429,7 +5429,7 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D278" t="inlineStr">
         <is>
@@ -5501,7 +5501,7 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D282" t="inlineStr">
         <is>
@@ -5951,7 +5951,7 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D307" t="inlineStr">
         <is>
@@ -6311,7 +6311,7 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D327" t="inlineStr">
         <is>
@@ -6329,7 +6329,7 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D328" t="inlineStr">
         <is>
@@ -6401,7 +6401,7 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D332" t="inlineStr">
         <is>
@@ -6473,7 +6473,7 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D336" t="inlineStr">
         <is>
@@ -6743,7 +6743,7 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D351" t="inlineStr">
         <is>
@@ -6833,7 +6833,7 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D356" t="inlineStr">
         <is>
@@ -7283,7 +7283,7 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="D381" t="inlineStr">
         <is>
@@ -7301,7 +7301,7 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D382" t="inlineStr">
         <is>
@@ -7373,7 +7373,7 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D386" t="inlineStr">
         <is>
@@ -7841,7 +7841,7 @@
         </is>
       </c>
       <c r="C412" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D412" t="inlineStr">
         <is>
@@ -7985,7 +7985,7 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D420" t="inlineStr">
         <is>
@@ -8201,7 +8201,7 @@
         </is>
       </c>
       <c r="C432" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D432" t="inlineStr">
         <is>

</xml_diff>